<commit_message>
Added docs to stk api
</commit_message>
<xml_diff>
--- a/Reports/PruebaObs.xlsx
+++ b/Reports/PruebaObs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,37 +436,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>y</t>
+          <t>C/No</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>Eb/No</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>xVel</t>
+          <t>BER</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>yVel</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>zVel</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>RelSpeed</t>
+          <t>Range</t>
         </is>
       </c>
     </row>
@@ -474,312 +464,264 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>3964.512409572058</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:29.000000000</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>861.342671279469</v>
+        <v>-2.94901106364583</v>
       </c>
       <c r="D2" t="n">
-        <v>-5712.700425888736</v>
+        <v>-5.959311020285641</v>
       </c>
       <c r="E2" t="n">
-        <v>6.211611579276539</v>
+        <v>0.238197132938244</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.4792013980275444</v>
-      </c>
-      <c r="G2" t="n">
-        <v>4.239321606546941</v>
-      </c>
-      <c r="H2" t="n">
-        <v>7.535622076206429</v>
+        <v>2754.089201487097</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>3970.721597992269</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:39.000000000</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>860.8629741816796</v>
+        <v>-28.15247928870762</v>
       </c>
       <c r="D3" t="n">
-        <v>-5708.457880310436</v>
+        <v>-31.16277924534743</v>
       </c>
       <c r="E3" t="n">
-        <v>6.207028539138427</v>
+        <v>0.4843981768018749</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.4801960788689023</v>
-      </c>
-      <c r="G3" t="n">
-        <v>4.245935847962363</v>
-      </c>
-      <c r="H3" t="n">
-        <v>7.535632872217957</v>
+        <v>2685.571758676042</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>3976.926200479859</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:49.000000000</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>860.3822797908863</v>
+        <v>-1.229907376169047</v>
       </c>
       <c r="D4" t="n">
-        <v>-5704.208723076426</v>
+        <v>-4.240207332808859</v>
       </c>
       <c r="E4" t="n">
-        <v>6.20243829683852</v>
+        <v>0.1927054244717706</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.4811902164894614</v>
-      </c>
-      <c r="G4" t="n">
-        <v>4.25254521762159</v>
-      </c>
-      <c r="H4" t="n">
-        <v>7.53564368043305</v>
+        <v>2617.106297974157</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>3983.126209228498</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:59.000000000</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>859.9005915549699</v>
+        <v>-10.14464047948895</v>
       </c>
       <c r="D5" t="n">
-        <v>-5699.952959046439</v>
+        <v>-13.15494043612876</v>
       </c>
       <c r="E5" t="n">
-        <v>6.197840857880742</v>
+        <v>0.3778982457374752</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.4821838052218105</v>
-      </c>
-      <c r="G5" t="n">
-        <v>4.259149707868335</v>
-      </c>
-      <c r="H5" t="n">
-        <v>7.535654500816038</v>
+        <v>2548.705801581525</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>3989.321616375719</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:16:09.000000000</t>
+        </is>
       </c>
       <c r="C6" t="n">
-        <v>859.4179129455696</v>
+        <v>-10.05917224203106</v>
       </c>
       <c r="D6" t="n">
-        <v>-5695.690593130985</v>
+        <v>-13.06947219867087</v>
       </c>
       <c r="E6" t="n">
-        <v>6.193236227826831</v>
+        <v>0.3767298360609527</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.4831768394029923</v>
-      </c>
-      <c r="G6" t="n">
-        <v>4.265749310984622</v>
-      </c>
-      <c r="H6" t="n">
-        <v>7.535665333331089</v>
+        <v>2480.3844497692</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>3995.512416012813</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:16:19.000000000</t>
+        </is>
       </c>
       <c r="C7" t="n">
-        <v>858.9342386780683</v>
+        <v>-6.540831652997997</v>
       </c>
       <c r="D7" t="n">
-        <v>-5691.421630205936</v>
+        <v>-9.55113160963781</v>
       </c>
       <c r="E7" t="n">
-        <v>6.188624411140019</v>
+        <v>0.3188445644709756</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.4841693269080649</v>
-      </c>
-      <c r="G7" t="n">
-        <v>4.272344019333244</v>
-      </c>
-      <c r="H7" t="n">
-        <v>7.535676177942448</v>
+        <v>2412.157784091685</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
-        <v>4001.698600313632</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:16:29.000000000</t>
+        </is>
       </c>
       <c r="C8" t="n">
-        <v>858.4495722193366</v>
+        <v>-19.53143848642713</v>
       </c>
       <c r="D8" t="n">
-        <v>-5687.146075179227</v>
+        <v>-22.54173844306695</v>
       </c>
       <c r="E8" t="n">
-        <v>6.184005413378698</v>
+        <v>0.4579726067351606</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.4851612620768703</v>
-      </c>
-      <c r="G8" t="n">
-        <v>4.278933825234578</v>
-      </c>
-      <c r="H8" t="n">
-        <v>7.535687034614274</v>
+        <v>2344.042903608837</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
-        <v>4007.880161489679</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:16:39.000000000</t>
+        </is>
       </c>
       <c r="C9" t="n">
-        <v>857.9639170545212</v>
+        <v>-1.744837658402866</v>
       </c>
       <c r="D9" t="n">
-        <v>-5682.863932944791</v>
+        <v>-4.755137615042678</v>
       </c>
       <c r="E9" t="n">
-        <v>6.179379240089308</v>
+        <v>0.2066760055034322</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.4861526392659572</v>
-      </c>
-      <c r="G9" t="n">
-        <v>4.285518721047661</v>
-      </c>
-      <c r="H9" t="n">
-        <v>7.535697903310743</v>
+        <v>2276.058681724883</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>4014.057093609343</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:16:49.000000000</t>
+        </is>
       </c>
       <c r="C10" t="n">
-        <v>857.477267877224</v>
+        <v>-7.388618359481662</v>
       </c>
       <c r="D10" t="n">
-        <v>-5678.575208426671</v>
+        <v>-10.39891831612147</v>
       </c>
       <c r="E10" t="n">
-        <v>6.174745895782975</v>
+        <v>0.3346390959397672</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.4871434663276014</v>
-      </c>
-      <c r="G10" t="n">
-        <v>4.292098699112019</v>
-      </c>
-      <c r="H10" t="n">
-        <v>7.535708783995932</v>
+        <v>2208.226032162438</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
-        <v>4020.229388883887</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:16:59.000000000</t>
+        </is>
       </c>
       <c r="C11" t="n">
-        <v>856.9896281704164</v>
+        <v>-0.8371421059926083</v>
       </c>
       <c r="D11" t="n">
-        <v>-5674.279906541334</v>
+        <v>-3.847442062632421</v>
       </c>
       <c r="E11" t="n">
-        <v>6.170105386029912</v>
+        <v>0.1819076049461735</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.488133737615651</v>
-      </c>
-      <c r="G11" t="n">
-        <v>4.298673751786031</v>
-      </c>
-      <c r="H11" t="n">
-        <v>7.535719676633954</v>
+        <v>2140.568221581015</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
-        <v>4026.39703952071</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:17:09.000000000</t>
+        </is>
       </c>
       <c r="C12" t="n">
-        <v>856.5010014374786</v>
+        <v>-2.838639365189925</v>
       </c>
       <c r="D12" t="n">
-        <v>-5669.978032220131</v>
+        <v>-5.848939321829737</v>
       </c>
       <c r="E12" t="n">
-        <v>6.165457716419422</v>
+        <v>0.2353869473907544</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.4891234474957289</v>
-      </c>
-      <c r="G12" t="n">
-        <v>4.305243871422255</v>
-      </c>
-      <c r="H12" t="n">
-        <v>7.535730581188846</v>
+        <v>2073.111225564506</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="n">
-        <v>4032.560039622659</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:17:19.000000000</t>
+        </is>
       </c>
       <c r="C13" t="n">
-        <v>856.011382346534</v>
+        <v>-3.892056142929642</v>
       </c>
       <c r="D13" t="n">
-        <v>-5665.669590395523</v>
+        <v>-6.902356099569453</v>
       </c>
       <c r="E13" t="n">
-        <v>6.160802891467719</v>
+        <v>0.2614610754993032</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.4901126038053054</v>
-      </c>
-      <c r="G13" t="n">
-        <v>4.311809050398241</v>
-      </c>
-      <c r="H13" t="n">
-        <v>7.535741497624637</v>
+        <v>2005.884170588258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>